<commit_message>
SfA model selection update
</commit_message>
<xml_diff>
--- a/results/SOA results/gamm_SOA_model_selection.xlsx
+++ b/results/SOA results/gamm_SOA_model_selection.xlsx
@@ -479,28 +479,28 @@
         <v>11</v>
       </c>
       <c r="C2" t="n">
-        <v>39.3271858672674</v>
+        <v>39.7741120585799</v>
       </c>
       <c r="D2" t="n">
-        <v>-4494.06405419129</v>
+        <v>-4446.38897826738</v>
       </c>
       <c r="E2" t="n">
-        <v>9070.95579067745</v>
+        <v>8976.28504729307</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0.971698107610557</v>
+        <v>1</v>
       </c>
       <c r="H2" t="n">
-        <v>9278.972051699</v>
+        <v>9186.00759785883</v>
       </c>
       <c r="I2" t="n">
-        <v>241351.712289256</v>
+        <v>212197.971105761</v>
       </c>
       <c r="J2" t="n">
-        <v>1082.67281413273</v>
+        <v>1082.22588794142</v>
       </c>
     </row>
     <row r="3">
@@ -520,10 +520,10 @@
         <v>9079.24652861638</v>
       </c>
       <c r="F3" t="n">
-        <v>8.2907379389344</v>
+        <v>102.961481323311</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0153893574812468</v>
+        <v>0.0000000000000000000000438731085200036</v>
       </c>
       <c r="H3" t="n">
         <v>9301.23054674478</v>
@@ -552,10 +552,10 @@
         <v>9079.59748393636</v>
       </c>
       <c r="F4" t="n">
-        <v>8.64169325891089</v>
+        <v>103.312436643288</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0129125349081967</v>
+        <v>0.0000000000000000000000368120011498852</v>
       </c>
       <c r="H4" t="n">
         <v>9301.27587562864</v>
@@ -584,10 +584,10 @@
         <v>9188.09374213157</v>
       </c>
       <c r="F5" t="n">
-        <v>117.137951454117</v>
+        <v>211.808694838493</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0000000000000000000000000355916717946782</v>
+        <v>0.000000000000000000000000000000000000000000000101467347220903</v>
       </c>
       <c r="H5" t="n">
         <v>9390.44619589228</v>
@@ -616,10 +616,10 @@
         <v>9251.97095479142</v>
       </c>
       <c r="F6" t="n">
-        <v>181.015164113966</v>
+        <v>275.685907498342</v>
       </c>
       <c r="G6" t="n">
-        <v>0.00000000000000000000000000000000000000047927844682333</v>
+        <v>0.00000000000000000000000000000000000000000000000000000000000136636213268829</v>
       </c>
       <c r="H6" t="n">
         <v>9444.61716557439</v>
@@ -648,10 +648,10 @@
         <v>9662.24516021475</v>
       </c>
       <c r="F7" t="n">
-        <v>591.289369537302</v>
+        <v>685.960112921679</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000038965132545005</v>
+        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000111084656440435</v>
       </c>
       <c r="H7" t="n">
         <v>9761.47184877672</v>
@@ -680,10 +680,10 @@
         <v>9689.10600798152</v>
       </c>
       <c r="F8" t="n">
-        <v>618.15021730407</v>
+        <v>712.820960688447</v>
       </c>
       <c r="G8" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000572686803487259</v>
+        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000163265752374575</v>
       </c>
       <c r="H8" t="n">
         <v>9777.77675037761</v>
@@ -712,10 +712,10 @@
         <v>9695.04747853099</v>
       </c>
       <c r="F9" t="n">
-        <v>624.091687853535</v>
+        <v>718.762431237912</v>
       </c>
       <c r="G9" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000293591338348731</v>
+        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000836991710901724</v>
       </c>
       <c r="H9" t="n">
         <v>9773.66880423057</v>
@@ -744,10 +744,10 @@
         <v>9747.01468906887</v>
       </c>
       <c r="F10" t="n">
-        <v>676.058898391422</v>
+        <v>770.729641775799</v>
       </c>
       <c r="G10" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000152477881892675</v>
+        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000434695124038125</v>
       </c>
       <c r="H10" t="n">
         <v>9820.09193900943</v>
@@ -776,10 +776,10 @@
         <v>10227.9773955505</v>
       </c>
       <c r="F11" t="n">
-        <v>1157.02160487309</v>
+        <v>1251.69234825747</v>
       </c>
       <c r="G11" t="n">
-        <v>5.53964758717002e-252</v>
+        <v>1.57928334597889e-272</v>
       </c>
       <c r="H11" t="n">
         <v>10263.1071762591</v>
@@ -808,10 +808,10 @@
         <v>10469.1089980534</v>
       </c>
       <c r="F12" t="n">
-        <v>1398.15320737594</v>
+        <v>1492.82395076031</v>
       </c>
       <c r="G12" t="n">
-        <v>2.41223685004431e-304</v>
+        <v>0</v>
       </c>
       <c r="H12" t="n">
         <v>10489.2004703977</v>

</xml_diff>